<commit_message>
fix xls. added descriptions, more participants, enh timing breakdown, fix typos
</commit_message>
<xml_diff>
--- a/surveyux/survey_eval.xlsx
+++ b/surveyux/survey_eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Githubs\IEEE-Technology-and-Society-Draft\surveyux\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61C8062-A3D7-4150-9415-66344C6AABD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F6CCBD-4078-4FAF-837A-D0E163F2A4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{D8488B4A-5A4F-4189-8080-6FE281BAE78B}"/>
+    <workbookView xWindow="30165" yWindow="2250" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{D8488B4A-5A4F-4189-8080-6FE281BAE78B}"/>
   </bookViews>
   <sheets>
     <sheet name="Likert Scale" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t>N = 7</t>
   </si>
@@ -180,6 +180,15 @@
       </rPr>
       <t>SD</t>
     </r>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P10</t>
   </si>
 </sst>
 </file>
@@ -234,10 +243,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -574,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC04A67-C47C-4C55-8D0A-24A0F0423417}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -848,86 +859,119 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="2">
-        <f>AVERAGE(B5:B11)</f>
+      <c r="B16" s="2">
+        <f>AVERAGE(B5:B14)</f>
         <v>4.7142857142857144</v>
       </c>
-      <c r="C12" s="2">
-        <f t="shared" ref="C12:J12" si="0">AVERAGE(C5:C11)</f>
+      <c r="C16" s="2">
+        <f t="shared" ref="C16:J16" si="0">AVERAGE(C5:C14)</f>
         <v>4.5714285714285712</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>1.8333333333333333</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E16" s="2">
         <f t="shared" si="0"/>
         <v>4.7142857142857144</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F16" s="2">
         <f t="shared" si="0"/>
         <v>4.7142857142857144</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G16" s="2">
         <f t="shared" si="0"/>
         <v>1.5714285714285714</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H16" s="2">
         <f t="shared" si="0"/>
         <v>4.4285714285714288</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I16" s="2">
         <f t="shared" si="0"/>
         <v>4.7142857142857144</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J16" s="2">
         <f t="shared" si="0"/>
         <v>4.4285714285714288</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="2">
-        <f>_xlfn.STDEV.S(B5:B12)</f>
-        <v>0.45175395145262559</v>
-      </c>
-      <c r="C13" s="2">
-        <f t="shared" ref="C13:J13" si="1">_xlfn.STDEV.S(C5:C12)</f>
-        <v>0.49487165930539467</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="B17" s="2">
+        <f>_xlfn.STDEV.S(B5:B14)</f>
+        <v>0.48795003647426655</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" ref="C17:J17" si="1">_xlfn.STDEV.S(C5:C14)</f>
+        <v>0.53452248382485001</v>
+      </c>
+      <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>0.89752746785575055</v>
-      </c>
-      <c r="E13" s="2">
+        <v>0.9831920802501749</v>
+      </c>
+      <c r="E17" s="2">
         <f t="shared" si="1"/>
-        <v>0.45175395145262559</v>
-      </c>
-      <c r="F13" s="2">
+        <v>0.48795003647426655</v>
+      </c>
+      <c r="F17" s="2">
         <f t="shared" si="1"/>
-        <v>0.45175395145262559</v>
-      </c>
-      <c r="G13" s="2">
+        <v>0.48795003647426655</v>
+      </c>
+      <c r="G17" s="2">
         <f t="shared" si="1"/>
-        <v>0.72843135908468359</v>
-      </c>
-      <c r="H13" s="2">
+        <v>0.7867957924694432</v>
+      </c>
+      <c r="H17" s="2">
         <f t="shared" si="1"/>
-        <v>0.49487165930539057</v>
-      </c>
-      <c r="I13" s="2">
+        <v>0.53452248382485001</v>
+      </c>
+      <c r="I17" s="2">
         <f t="shared" si="1"/>
-        <v>0.45175395145262565</v>
-      </c>
-      <c r="J13" s="2">
+        <v>0.48795003647426666</v>
+      </c>
+      <c r="J17" s="2">
         <f t="shared" si="1"/>
-        <v>0.7284313590846816</v>
+        <v>0.78679579246944398</v>
       </c>
     </row>
   </sheetData>
@@ -938,10 +982,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6A12C1-567F-4693-910A-8AC58E4581FB}">
-  <dimension ref="A4:D11"/>
+  <dimension ref="A4:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1063,6 +1107,21 @@
         <v>19</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>